<commit_message>
längsstreben eingefügt, winkel konstruiert
</commit_message>
<xml_diff>
--- a/Projekt/Zeichenmaschine_v2/weitere Dateien/Parameter_1.xlsx
+++ b/Projekt/Zeichenmaschine_v2/weitere Dateien/Parameter_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\DrawMachine\DrawMachineConstruction\Projekt\Zeichenmaschine_v2\weitere Dateien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B852D88C-6437-4C17-8414-9034DE950727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFDC2CD-A807-46C7-863A-6DAC60C6C62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <t>Parametername</t>
   </si>
@@ -146,6 +146,30 @@
   </si>
   <si>
     <t>GM_Platte_Höhe</t>
+  </si>
+  <si>
+    <t>Rundung_Platte</t>
+  </si>
+  <si>
+    <t>GM_Schrauben_Pos_Abstand_kurz</t>
+  </si>
+  <si>
+    <t>GM_Schrauben_Pos_Abstand_lang</t>
+  </si>
+  <si>
+    <t>GM_Stift_Durchmesser</t>
+  </si>
+  <si>
+    <t>GM_Schrauben_Pos_Stift_rlang</t>
+  </si>
+  <si>
+    <t>GM_Schrauben_Pos_Stift_rkurz</t>
+  </si>
+  <si>
+    <t>m2,5</t>
+  </si>
+  <si>
+    <t>GM_Schrauben_Durchgangsloch</t>
   </si>
 </sst>
 </file>
@@ -161,12 +185,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -181,8 +211,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -497,21 +528,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="42.88671875" customWidth="1"/>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -525,7 +556,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -539,7 +570,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -553,7 +584,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -567,7 +598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -581,7 +612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -595,7 +626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -606,7 +637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -617,7 +648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -628,7 +659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -639,7 +670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -650,18 +681,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12">
-        <v>160</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <v>150</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -672,7 +703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -683,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -694,7 +725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -705,7 +736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -716,7 +747,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -727,7 +758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -738,7 +769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -749,7 +780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -760,7 +791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -771,7 +802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -782,7 +813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -793,7 +824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -804,7 +835,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -815,7 +846,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -826,7 +857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -834,6 +865,86 @@
         <v>20</v>
       </c>
       <c r="C28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30">
+        <v>18.37</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31">
+        <v>34.369999999999997</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34">
+        <v>9.1850000000000005</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35">
+        <v>2.7</v>
+      </c>
+      <c r="C35" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
gerüst von item importiert, dateien sortiert, issue: ordner schreibfehler korriegieren, baugruppe mit motoren und netzteil und platte und gerüst erstellen
</commit_message>
<xml_diff>
--- a/Projekt/Zeichenmaschine_v2/weitere Dateien/Parameter_1.xlsx
+++ b/Projekt/Zeichenmaschine_v2/weitere Dateien/Parameter_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\DrawMachine\DrawMachineConstruction\Projekt\Zeichenmaschine_v2\weitere Dateien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFDC2CD-A807-46C7-863A-6DAC60C6C62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060D24DA-B10D-4DEE-B49E-E43F783D29F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -531,7 +531,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>